<commit_message>
ajout config ip des appareils
changement nom des screenshots laptops
</commit_message>
<xml_diff>
--- a/Materiel/liste_materiel.xlsx
+++ b/Materiel/liste_materiel.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21390" windowHeight="8025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21390" windowHeight="8025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inventaire" sheetId="1" r:id="rId1"/>
+    <sheet name="configuration IPv4" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Liste Matériel</t>
   </si>
@@ -59,14 +60,86 @@
     <t>S/FTP cat 6a</t>
   </si>
   <si>
-    <t>Wireless AP</t>
+    <t>laptops Dell</t>
+  </si>
+  <si>
+    <t>router Dlink</t>
+  </si>
+  <si>
+    <t>SXT</t>
+  </si>
+  <si>
+    <t>dlink</t>
+  </si>
+  <si>
+    <t>OmniTik1</t>
+  </si>
+  <si>
+    <t>OmniTik2</t>
+  </si>
+  <si>
+    <t>OmniTik3</t>
+  </si>
+  <si>
+    <t>SXT1</t>
+  </si>
+  <si>
+    <t>SXT2</t>
+  </si>
+  <si>
+    <t>SXT3</t>
+  </si>
+  <si>
+    <t>nom appareil</t>
+  </si>
+  <si>
+    <t>type appareil</t>
+  </si>
+  <si>
+    <t>adresse IPv4</t>
+  </si>
+  <si>
+    <t>192.168.0.50</t>
+  </si>
+  <si>
+    <t>192.168.0.30</t>
+  </si>
+  <si>
+    <t>192.168.0.31</t>
+  </si>
+  <si>
+    <t>192.168.0.32</t>
+  </si>
+  <si>
+    <t>192.168.0.40</t>
+  </si>
+  <si>
+    <t>192.168.0.41</t>
+  </si>
+  <si>
+    <t>192.168.0.42</t>
+  </si>
+  <si>
+    <t>192.168.0.20</t>
+  </si>
+  <si>
+    <t>192.168.0.21</t>
+  </si>
+  <si>
+    <t>Wireless AP dlink</t>
+  </si>
+  <si>
+    <t>SC-C111-LP23</t>
+  </si>
+  <si>
+    <t>SC-C111-LP17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,8 +147,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,8 +175,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -118,22 +205,213 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,17 +705,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>2</v>
       </c>
     </row>
@@ -445,7 +723,7 @@
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>2</v>
       </c>
     </row>
@@ -453,7 +731,7 @@
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
     </row>
@@ -461,7 +739,7 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
     </row>
@@ -469,7 +747,7 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>3</v>
       </c>
     </row>
@@ -477,7 +755,7 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>3</v>
       </c>
     </row>
@@ -485,7 +763,7 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>6</v>
       </c>
     </row>
@@ -493,7 +771,7 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>1</v>
       </c>
     </row>
@@ -501,7 +779,7 @@
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>1</v>
       </c>
     </row>
@@ -509,15 +787,15 @@
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5">
+        <v>33</v>
+      </c>
+      <c r="B12" s="4">
         <v>1</v>
       </c>
     </row>
@@ -528,4 +806,156 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="18"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>